<commit_message>
se cambian stats de velocidad y velocidad de ataue para dar más balance al juego
</commit_message>
<xml_diff>
--- a/docs/RPG semiturnos (versión 1).xlsx
+++ b/docs/RPG semiturnos (versión 1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="38380" windowHeight="20320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="38380" windowHeight="20320" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="pasivas" sheetId="2" r:id="rId1"/>
@@ -12822,8 +12822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12913,13 +12913,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="2">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="D4" s="49" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" s="47" t="s">
         <v>21</v>
@@ -14460,7 +14460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N423"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+    <sheetView topLeftCell="A241" workbookViewId="0">
       <selection activeCell="G258" sqref="G258"/>
     </sheetView>
   </sheetViews>
@@ -27341,7 +27341,7 @@
   <dimension ref="A1:AO133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="S45" sqref="S45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -40887,7 +40887,7 @@
   <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -41126,13 +41126,13 @@
       </c>
       <c r="D7" s="2">
         <f>$D$1*(0.45*E7+0.3*F7+0.35*G7+0.6325*H7*O7+0.3*K7+0.2*J7)</f>
-        <v>2703.5225</v>
+        <v>2780.1724999999997</v>
       </c>
       <c r="E7" s="2">
         <v>-20</v>
       </c>
       <c r="F7" s="2">
-        <v>-11.2</v>
+        <v>-3.9</v>
       </c>
       <c r="G7" s="2">
         <v>-60</v>
@@ -41175,13 +41175,13 @@
       </c>
       <c r="D8" s="2">
         <f t="shared" ref="D8:D54" si="0">$D$1*(0.45*E8+0.3*F8+0.35*G8+0.6325*H8*O8+0.3*K8+0.2*J8)</f>
-        <v>4053.8312499999993</v>
+        <v>4105.2812499999991</v>
       </c>
       <c r="E8" s="2">
         <v>-10</v>
       </c>
       <c r="F8" s="2">
-        <v>-7.5</v>
+        <v>-2.6</v>
       </c>
       <c r="G8" s="2">
         <v>-32</v>
@@ -41225,13 +41225,13 @@
       <c r="C9" s="56"/>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>4225.0687499999995</v>
+        <v>4288.0687499999995</v>
       </c>
       <c r="E9" s="2">
         <v>-10</v>
       </c>
       <c r="F9" s="2">
-        <v>-9.4</v>
+        <v>-3.4</v>
       </c>
       <c r="G9" s="2">
         <v>-43.5</v>
@@ -41274,13 +41274,13 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>4521.3218749999996</v>
+        <v>4547.5718749999996</v>
       </c>
       <c r="E10" s="2">
         <v>-5</v>
       </c>
       <c r="F10" s="2">
-        <v>-3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G10" s="2">
         <v>-14.5</v>
@@ -41324,13 +41324,13 @@
       <c r="C11" s="56"/>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>4376.2687500000002</v>
+        <v>4414.0687500000004</v>
       </c>
       <c r="E11" s="2">
         <v>-5</v>
       </c>
       <c r="F11" s="2">
-        <v>-5.6</v>
+        <v>-2</v>
       </c>
       <c r="G11" s="2">
         <v>-30</v>
@@ -41371,13 +41371,13 @@
       <c r="C12" s="56"/>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>4372.0031249999993</v>
+        <v>4398.2531249999993</v>
       </c>
       <c r="E12" s="2">
         <v>-5</v>
       </c>
       <c r="F12" s="2">
-        <v>-3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G12" s="2">
         <v>-12</v>
@@ -41420,13 +41420,13 @@
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>2431.5549999999998</v>
+        <v>2457.8049999999998</v>
       </c>
       <c r="E13" s="2">
         <v>-5</v>
       </c>
       <c r="F13" s="2">
-        <v>-3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G13" s="2">
         <v>-60</v>
@@ -41467,13 +41467,13 @@
       <c r="C14" s="56"/>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>2994.2849999999999</v>
+        <v>3006.8850000000002</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>-1.9</v>
+        <v>-0.7</v>
       </c>
       <c r="G14" s="2">
         <v>-12</v>
@@ -41514,13 +41514,13 @@
       <c r="C15" s="56"/>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>2599.66</v>
+        <v>2612.2599999999998</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
       </c>
       <c r="F15" s="2">
-        <v>-1.9</v>
+        <v>-0.7</v>
       </c>
       <c r="G15" s="2">
         <v>-23.2</v>
@@ -41561,13 +41561,13 @@
       <c r="C16" s="56"/>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>3281.9499999999994</v>
+        <v>3333.3999999999992</v>
       </c>
       <c r="E16" s="2">
         <v>-10</v>
       </c>
       <c r="F16" s="2">
-        <v>-7.5</v>
+        <v>-2.6</v>
       </c>
       <c r="G16" s="2">
         <v>-67</v>
@@ -41896,13 +41896,13 @@
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>2685.4012500000003</v>
+        <v>2723.2012500000001</v>
       </c>
       <c r="E23" s="2">
         <v>-10</v>
       </c>
       <c r="F23" s="2">
-        <v>-5.6</v>
+        <v>-2</v>
       </c>
       <c r="G23" s="2">
         <v>-14.5</v>
@@ -41943,13 +41943,13 @@
       <c r="C24" s="58"/>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>2052.5924999999997</v>
+        <v>2078.8424999999997</v>
       </c>
       <c r="E24" s="2">
         <v>-5</v>
       </c>
       <c r="F24" s="2">
-        <v>-3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G24" s="2">
         <v>-6</v>
@@ -42276,13 +42276,13 @@
       <c r="C31" s="56"/>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>4191.915</v>
+        <v>4202.415</v>
       </c>
       <c r="E31" s="2">
         <v>20</v>
       </c>
       <c r="F31" s="2">
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="G31" s="2">
         <v>12</v>
@@ -42323,13 +42323,13 @@
       <c r="C32" s="56"/>
       <c r="D32" s="2">
         <f t="shared" si="0"/>
-        <v>3972.8150000000005</v>
+        <v>3985.4150000000004</v>
       </c>
       <c r="E32" s="2">
         <v>-5</v>
       </c>
       <c r="F32" s="2">
-        <v>-1.9</v>
+        <v>-0.7</v>
       </c>
       <c r="G32" s="2">
         <v>-14.5</v>
@@ -42513,13 +42513,13 @@
       </c>
       <c r="D36" s="2">
         <f t="shared" si="0"/>
-        <v>2870.6824999999999</v>
+        <v>2883.2824999999998</v>
       </c>
       <c r="E36" s="2">
         <v>0</v>
       </c>
       <c r="F36" s="2">
-        <v>-1.9</v>
+        <v>-0.7</v>
       </c>
       <c r="G36" s="2">
         <v>-14.5</v>
@@ -42560,13 +42560,13 @@
       <c r="C37" s="56"/>
       <c r="D37" s="2">
         <f t="shared" si="0"/>
-        <v>1999.6024999999995</v>
+        <v>2025.8524999999993</v>
       </c>
       <c r="E37" s="2">
         <v>0</v>
       </c>
       <c r="F37" s="2">
-        <v>-3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G37" s="2">
         <v>-43.5</v>
@@ -42609,13 +42609,13 @@
       </c>
       <c r="D38" s="2">
         <f t="shared" si="0"/>
-        <v>50.750000000000007</v>
+        <v>58.100000000000009</v>
       </c>
       <c r="E38" s="2">
         <v>15</v>
       </c>
       <c r="F38" s="2">
-        <v>-1</v>
+        <v>-0.3</v>
       </c>
       <c r="G38" s="2">
         <v>-10</v>
@@ -42654,13 +42654,13 @@
       <c r="C39" s="56"/>
       <c r="D39" s="2">
         <f t="shared" si="0"/>
-        <v>102.54999999999998</v>
+        <v>115.14999999999998</v>
       </c>
       <c r="E39" s="2">
         <v>30</v>
       </c>
       <c r="F39" s="2">
-        <v>-1.9</v>
+        <v>-0.7</v>
       </c>
       <c r="G39" s="2">
         <v>-20</v>
@@ -42699,13 +42699,13 @@
       <c r="C40" s="56"/>
       <c r="D40" s="2">
         <f t="shared" si="0"/>
-        <v>93.45000000000006</v>
+        <v>117.59999999999998</v>
       </c>
       <c r="E40" s="2">
         <v>45</v>
       </c>
       <c r="F40" s="2">
-        <v>-3.6</v>
+        <v>-1.3</v>
       </c>
       <c r="G40" s="2">
         <v>-30</v>
@@ -42748,13 +42748,13 @@
       </c>
       <c r="D41" s="2">
         <f t="shared" si="0"/>
-        <v>1494.9374999999998</v>
+        <v>1523.2874999999997</v>
       </c>
       <c r="E41" s="2">
         <v>-5</v>
       </c>
       <c r="F41" s="2">
-        <v>-4.2</v>
+        <v>-1.5</v>
       </c>
       <c r="G41" s="2">
         <v>-36</v>
@@ -42795,13 +42795,13 @@
       <c r="C42" s="56"/>
       <c r="D42" s="2">
         <f t="shared" si="0"/>
-        <v>1746.5874999999996</v>
+        <v>1772.8374999999996</v>
       </c>
       <c r="E42" s="2">
         <v>-5</v>
       </c>
       <c r="F42" s="2">
-        <v>-3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G42" s="2">
         <v>-15.8</v>
@@ -42842,13 +42842,13 @@
       <c r="C43" s="56"/>
       <c r="D43" s="2">
         <f t="shared" si="0"/>
-        <v>1746.5874999999996</v>
+        <v>1772.8374999999996</v>
       </c>
       <c r="E43" s="2">
         <v>-5</v>
       </c>
       <c r="F43" s="2">
-        <v>-3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G43" s="2">
         <v>-15.8</v>
@@ -42891,13 +42891,13 @@
       </c>
       <c r="D44" s="2">
         <f t="shared" si="0"/>
-        <v>5934.4250000000002</v>
+        <v>5960.6750000000002</v>
       </c>
       <c r="E44" s="2">
         <v>-5</v>
       </c>
       <c r="F44" s="2">
-        <v>-3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G44" s="2">
         <v>-95</v>
@@ -43083,13 +43083,13 @@
       </c>
       <c r="D48" s="2">
         <f t="shared" si="0"/>
-        <v>10809.224999999997</v>
+        <v>10872.224999999999</v>
       </c>
       <c r="E48" s="2">
         <v>-10</v>
       </c>
       <c r="F48" s="2">
-        <v>-9.4</v>
+        <v>-3.4</v>
       </c>
       <c r="G48" s="2">
         <v>-134</v>
@@ -43130,13 +43130,13 @@
       <c r="C49" s="56"/>
       <c r="D49" s="2">
         <f t="shared" si="0"/>
-        <v>9353.0500000000011</v>
+        <v>9379.3000000000011</v>
       </c>
       <c r="E49" s="2">
         <v>-5</v>
       </c>
       <c r="F49" s="2">
-        <v>-3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G49" s="2">
         <v>-87</v>
@@ -43177,13 +43177,13 @@
       <c r="C50" s="56"/>
       <c r="D50" s="2">
         <f>$D$1*(0.45*E50+0.3*F50+0.35*G50+2.53*H50*O50+0.3*K50+0.2*J50)</f>
-        <v>10876.6875</v>
+        <v>10928.137499999999</v>
       </c>
       <c r="E50" s="2">
         <v>-10</v>
       </c>
       <c r="F50" s="2">
-        <v>-7.5</v>
+        <v>-2.6</v>
       </c>
       <c r="G50" s="2">
         <v>-150</v>
@@ -43273,13 +43273,13 @@
       <c r="C52" s="56"/>
       <c r="D52" s="2">
         <f t="shared" si="0"/>
-        <v>8177.5224999999973</v>
+        <v>8203.7724999999973</v>
       </c>
       <c r="E52" s="2">
         <v>0</v>
       </c>
       <c r="F52" s="2">
-        <v>-3.8</v>
+        <v>-1.3</v>
       </c>
       <c r="G52" s="2">
         <v>-55.3</v>
@@ -43320,13 +43320,13 @@
       <c r="C53" s="56"/>
       <c r="D53" s="2">
         <f t="shared" si="0"/>
-        <v>5875.1699999999992</v>
+        <v>5967.57</v>
       </c>
       <c r="E53" s="2">
         <v>-10</v>
       </c>
       <c r="F53" s="2">
-        <v>-10</v>
+        <v>-1.2</v>
       </c>
       <c r="G53" s="2">
         <v>-44</v>
@@ -43443,7 +43443,7 @@
   <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -45253,16 +45253,16 @@
       <c r="D49" s="56"/>
       <c r="E49" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8280</v>
       </c>
       <c r="F49" s="2">
         <v>0</v>
       </c>
       <c r="G49" s="2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H49" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I49" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
se generaliza creación de areaBox y su derivadas
</commit_message>
<xml_diff>
--- a/docs/RPG semiturnos (versión 1).xlsx
+++ b/docs/RPG semiturnos (versión 1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="38380" windowHeight="20320" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="38380" windowHeight="20320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cambios de estado" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6607" uniqueCount="2864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6608" uniqueCount="2865">
   <si>
     <t>Heroes</t>
   </si>
@@ -8583,9 +8583,6 @@
     <t>(0: =, 1: &lt;, 2: &lt;=, 3: &gt;, 4: &gt;=)</t>
   </si>
   <si>
-    <t>condicionado</t>
-  </si>
-  <si>
     <t>backstabTriggered(expr)</t>
   </si>
   <si>
@@ -8908,6 +8905,12 @@
   </si>
   <si>
     <t>60+6n</t>
+  </si>
+  <si>
+    <t>por pasivas</t>
+  </si>
+  <si>
+    <t>otras condiciones</t>
   </si>
 </sst>
 </file>
@@ -11066,8 +11069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11221,7 +11224,7 @@
         <v>1482</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2119</v>
@@ -11248,7 +11251,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -11285,7 +11288,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="32" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>2093</v>
@@ -11306,7 +11309,7 @@
         <v>1487</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>2124</v>
@@ -11322,7 +11325,7 @@
         <v>1488</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>2125</v>
@@ -11341,7 +11344,7 @@
         <v>2094</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>2160</v>
@@ -11405,7 +11408,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="32" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>2100</v>
@@ -11425,7 +11428,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="32" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>2105</v>
@@ -11445,7 +11448,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="32" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>2101</v>
@@ -11465,7 +11468,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="32" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>2102</v>
@@ -11485,7 +11488,7 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="32" t="s">
-        <v>2780</v>
+        <v>2779</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>2617</v>
@@ -11505,7 +11508,7 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="32" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>2103</v>
@@ -11525,7 +11528,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="32" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>2104</v>
@@ -11581,16 +11584,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>303</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>2162</v>
@@ -11599,16 +11602,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>2162</v>
@@ -11617,13 +11620,13 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="32" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>2846</v>
+        <v>2845</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>2160</v>
@@ -11649,7 +11652,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="32" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>2108</v>
@@ -11667,7 +11670,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>2107</v>
@@ -11685,16 +11688,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
+        <v>2826</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>2827</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>2828</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>2829</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>2830</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>2162</v>
@@ -11703,7 +11706,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>2786</v>
+        <v>2785</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>2109</v>
@@ -11721,7 +11724,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="32" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>2167</v>
@@ -11741,7 +11744,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="32" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>2096</v>
@@ -11759,7 +11762,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>2039</v>
@@ -11777,7 +11780,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>2110</v>
@@ -11795,7 +11798,7 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>2111</v>
@@ -11813,7 +11816,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>2040</v>
@@ -11831,7 +11834,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>2041</v>
@@ -11849,7 +11852,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>2042</v>
@@ -11867,7 +11870,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>2043</v>
@@ -11885,7 +11888,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>2044</v>
@@ -11903,7 +11906,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>2045</v>
@@ -11921,7 +11924,7 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>2046</v>
@@ -11939,7 +11942,7 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>2047</v>
@@ -11957,7 +11960,7 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>2038</v>
@@ -11975,7 +11978,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>2048</v>
@@ -11993,7 +11996,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>2049</v>
@@ -12011,13 +12014,13 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
+        <v>2834</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>2835</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>2836</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>2837</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>2171</v>
@@ -12029,7 +12032,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>2050</v>
@@ -12047,7 +12050,7 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>2051</v>
@@ -12065,13 +12068,13 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2" t="s">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>2771</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>2772</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>2773</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>2171</v>
@@ -12086,7 +12089,7 @@
         <v>2270</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>2269</v>
@@ -12117,7 +12120,7 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>2159</v>
@@ -12204,7 +12207,7 @@
         <v>-3</v>
       </c>
       <c r="D67" t="s">
-        <v>2755</v>
+        <v>2863</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -12214,6 +12217,12 @@
       <c r="B68" t="s">
         <v>2197</v>
       </c>
+      <c r="C68">
+        <v>-4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>2864</v>
+      </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
@@ -12399,7 +12408,7 @@
         <v>2213</v>
       </c>
       <c r="D91" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -12492,10 +12501,10 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
       <c r="B103" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -12623,82 +12632,82 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
+        <v>2755</v>
+      </c>
+      <c r="B119" t="s">
         <v>2756</v>
-      </c>
-      <c r="B119" t="s">
-        <v>2757</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
+        <v>2759</v>
+      </c>
+      <c r="B120" t="s">
         <v>2760</v>
-      </c>
-      <c r="B120" t="s">
-        <v>2761</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
+        <v>2765</v>
+      </c>
+      <c r="B121" t="s">
         <v>2766</v>
-      </c>
-      <c r="B121" t="s">
-        <v>2767</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
+        <v>2769</v>
+      </c>
+      <c r="B122" t="s">
         <v>2770</v>
-      </c>
-      <c r="B122" t="s">
-        <v>2771</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
+        <v>2820</v>
+      </c>
+      <c r="B123" t="s">
         <v>2821</v>
-      </c>
-      <c r="B123" t="s">
-        <v>2822</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B124" t="s">
         <v>2823</v>
-      </c>
-      <c r="B124" t="s">
-        <v>2824</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
+        <v>2830</v>
+      </c>
+      <c r="B125" t="s">
         <v>2831</v>
-      </c>
-      <c r="B125" t="s">
-        <v>2832</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
+        <v>2832</v>
+      </c>
+      <c r="B126" t="s">
         <v>2833</v>
-      </c>
-      <c r="B126" t="s">
-        <v>2834</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
+        <v>2854</v>
+      </c>
+      <c r="B127" t="s">
         <v>2855</v>
-      </c>
-      <c r="B127" t="s">
-        <v>2856</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
+        <v>2856</v>
+      </c>
+      <c r="B128" t="s">
         <v>2857</v>
-      </c>
-      <c r="B128" t="s">
-        <v>2858</v>
       </c>
     </row>
   </sheetData>
@@ -12719,7 +12728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -14391,10 +14400,10 @@
         <v>2534</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -14402,7 +14411,7 @@
         <v>2552</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2058</v>
@@ -14413,10 +14422,10 @@
         <v>343</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -14424,7 +14433,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>121</v>
@@ -14435,7 +14444,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>2774</v>
+        <v>2773</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>2227</v>
@@ -14446,7 +14455,7 @@
         <v>747</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2056</v>
@@ -14457,7 +14466,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2054</v>
@@ -14468,7 +14477,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>2817</v>
+        <v>2816</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2054</v>
@@ -14490,7 +14499,7 @@
         <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>2818</v>
+        <v>2817</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2059</v>
@@ -14501,7 +14510,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>2819</v>
+        <v>2818</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2060</v>
@@ -14512,10 +14521,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>2820</v>
+        <v>2819</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -14523,7 +14532,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>121</v>
@@ -14589,7 +14598,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>2057</v>
@@ -14600,7 +14609,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>2839</v>
+        <v>2838</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>2062</v>
@@ -14611,7 +14620,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>2063</v>
@@ -14759,7 +14768,7 @@
         <v>1518</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>2306</v>
@@ -14828,7 +14837,7 @@
         <v>130</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="C45" s="57" t="s">
         <v>1</v>
@@ -16237,11 +16246,6 @@
     <row r="150" spans="1:5" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C110:C114"/>
-    <mergeCell ref="C115:C119"/>
-    <mergeCell ref="C120:C124"/>
-    <mergeCell ref="C125:C129"/>
-    <mergeCell ref="C130:C134"/>
     <mergeCell ref="C145:C149"/>
     <mergeCell ref="C45:C49"/>
     <mergeCell ref="C50:C54"/>
@@ -16258,6 +16262,11 @@
     <mergeCell ref="C100:C104"/>
     <mergeCell ref="C105:C109"/>
     <mergeCell ref="C135:C139"/>
+    <mergeCell ref="C110:C114"/>
+    <mergeCell ref="C115:C119"/>
+    <mergeCell ref="C120:C124"/>
+    <mergeCell ref="C125:C129"/>
+    <mergeCell ref="C130:C134"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -16273,8 +16282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N423"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B43"/>
+    <sheetView topLeftCell="A380" workbookViewId="0">
+      <selection activeCell="K410" sqref="K410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16335,7 +16344,7 @@
         <v>294</v>
       </c>
       <c r="N3" t="s">
-        <v>2852</v>
+        <v>2851</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -16623,7 +16632,7 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>39</v>
@@ -16818,7 +16827,7 @@
         <v>4</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>127</v>
@@ -16996,7 +17005,7 @@
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="2" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="L23" s="7" t="s">
         <v>295</v>
@@ -24160,7 +24169,7 @@
         <v>5</v>
       </c>
       <c r="G258" s="2" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="H258" s="2" t="s">
         <v>127</v>
@@ -29105,7 +29114,7 @@
         <v>118</v>
       </c>
       <c r="F423" s="7" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="G423" s="2" t="s">
         <v>334</v>
@@ -29122,15 +29131,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B164:B183"/>
-    <mergeCell ref="B144:B163"/>
-    <mergeCell ref="B104:B123"/>
-    <mergeCell ref="B4:B23"/>
-    <mergeCell ref="B44:B63"/>
-    <mergeCell ref="B24:B43"/>
-    <mergeCell ref="B64:B83"/>
-    <mergeCell ref="B84:B103"/>
-    <mergeCell ref="B124:B143"/>
     <mergeCell ref="B384:B403"/>
     <mergeCell ref="B364:B383"/>
     <mergeCell ref="B184:B203"/>
@@ -29143,6 +29143,15 @@
     <mergeCell ref="B264:B283"/>
     <mergeCell ref="B224:B243"/>
     <mergeCell ref="B284:B303"/>
+    <mergeCell ref="B164:B183"/>
+    <mergeCell ref="B144:B163"/>
+    <mergeCell ref="B104:B123"/>
+    <mergeCell ref="B4:B23"/>
+    <mergeCell ref="B44:B63"/>
+    <mergeCell ref="B24:B43"/>
+    <mergeCell ref="B64:B83"/>
+    <mergeCell ref="B84:B103"/>
+    <mergeCell ref="B124:B143"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -29790,7 +29799,7 @@
         <v>1558</v>
       </c>
       <c r="AE9" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="AF9">
         <v>5</v>
@@ -32030,7 +32039,7 @@
         <v>1558</v>
       </c>
       <c r="AE45" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="46" spans="1:31">
@@ -41857,7 +41866,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="E3" t="s">
         <v>127</v>
@@ -45228,6 +45237,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B4:B18"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C29:C35"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="B41:B54"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="B19:B40"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="C8:C9"/>
@@ -45235,18 +45256,6 @@
     <mergeCell ref="C13:C18"/>
     <mergeCell ref="C19:C22"/>
     <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="B41:B54"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="B19:B40"/>
-    <mergeCell ref="B4:B18"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C29:C35"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C23:C25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -45552,7 +45561,7 @@
       </c>
       <c r="M7" s="2"/>
       <c r="P7" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="8" spans="1:16">

</xml_diff>